<commit_message>
A large batch of fixes to input excel
</commit_message>
<xml_diff>
--- a/src_files/unitdata_additional-vre.xlsx
+++ b/src_files/unitdata_additional-vre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728C47B8-B859-4FE8-B145-EAF8EF1C13E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE047157-531E-441B-8C3E-0CE7637100A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitdata" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -189,6 +217,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F36620C7-20BA-4A3D-A67B-523AEDE1C9AB}" name="Table1" displayName="Table1" ref="A1:F109" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
+  <autoFilter ref="A1:F109" xr:uid="{F36620C7-20BA-4A3D-A67B-523AEDE1C9AB}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E2B4C304-1D16-4618-BE09-796CC02CFF09}" name="Country"/>
+    <tableColumn id="2" xr3:uid="{CFD5C08B-CCCF-4A3D-96E2-35D2AD425B93}" name="Generator_ID"/>
+    <tableColumn id="3" xr3:uid="{AB2E3F07-003D-42B2-8F14-69E9DAF76CF7}" name="Scenario"/>
+    <tableColumn id="4" xr3:uid="{669744D3-508D-4EF8-96C9-CC14A535DEC4}" name="Year"/>
+    <tableColumn id="5" xr3:uid="{9283782A-59B9-40DC-AF37-EF8E6BBEF346}" name="capacity_output1"/>
+    <tableColumn id="6" xr3:uid="{B51875E4-A38D-4EC3-B717-A2DB36F684B2}" name="Note"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -304,14 +347,14 @@
   <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -2183,5 +2226,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>